<commit_message>
alterado os caminhos das pstas
</commit_message>
<xml_diff>
--- a/relatórios/relatorio.xlsx
+++ b/relatórios/relatorio.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M13"/>
+  <dimension ref="A1:M34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,36 +507,36 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>IN0006</t>
+          <t>IN0002</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Item 6</t>
+          <t>Item 2</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Descr 6</t>
+          <t>Descr 2</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>11</v>
+        <v>93</v>
       </c>
       <c r="G2" t="n">
-        <v>5</v>
+        <v>132</v>
       </c>
       <c r="H2" t="n">
-        <v>55</v>
+        <v>12276</v>
       </c>
       <c r="I2" t="n">
-        <v>9</v>
+        <v>231</v>
       </c>
       <c r="J2" t="n">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="K2" t="n">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="inlineStr"/>
@@ -544,40 +544,40 @@
     <row r="3">
       <c r="A3" t="inlineStr"/>
       <c r="B3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>IN0012</t>
+          <t>IN0003</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Item 12</t>
+          <t>Item 3</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Descr 12</t>
+          <t>Descr 3</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>18</v>
+        <v>57</v>
       </c>
       <c r="G3" t="n">
-        <v>22</v>
+        <v>151</v>
       </c>
       <c r="H3" t="n">
-        <v>396</v>
+        <v>8607</v>
       </c>
       <c r="I3" t="n">
-        <v>36</v>
+        <v>114</v>
       </c>
       <c r="J3" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K3" t="n">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
@@ -585,37 +585,37 @@
     <row r="4">
       <c r="A4" t="inlineStr"/>
       <c r="B4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>IN0018</t>
+          <t>IN0005</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Item 18</t>
+          <t>Item 5</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Descr 18</t>
+          <t>Descr 5</t>
         </is>
       </c>
       <c r="F4" t="n">
+        <v>75</v>
+      </c>
+      <c r="G4" t="n">
+        <v>62</v>
+      </c>
+      <c r="H4" t="n">
+        <v>4650</v>
+      </c>
+      <c r="I4" t="n">
+        <v>39</v>
+      </c>
+      <c r="J4" t="n">
         <v>12</v>
-      </c>
-      <c r="G4" t="n">
-        <v>6</v>
-      </c>
-      <c r="H4" t="n">
-        <v>72</v>
-      </c>
-      <c r="I4" t="n">
-        <v>7</v>
-      </c>
-      <c r="J4" t="n">
-        <v>13</v>
       </c>
       <c r="K4" t="n">
         <v>50</v>
@@ -630,36 +630,36 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>IN0025</t>
+          <t>IN0009</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Item 25</t>
+          <t>Item 9</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Descr 25</t>
+          <t>Descr 9</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>14</v>
+        <v>59</v>
       </c>
       <c r="G5" t="n">
-        <v>28</v>
+        <v>122</v>
       </c>
       <c r="H5" t="n">
-        <v>392</v>
+        <v>7198</v>
       </c>
       <c r="I5" t="n">
-        <v>21</v>
+        <v>82</v>
       </c>
       <c r="J5" t="n">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="K5" t="n">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="L5" t="inlineStr"/>
       <c r="M5" t="inlineStr"/>
@@ -671,33 +671,33 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>IN0006</t>
+          <t>IN0010</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Item 6</t>
+          <t>Item 10</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Descr 6</t>
+          <t>Descr 10</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="G6" t="n">
-        <v>5</v>
+        <v>175</v>
       </c>
       <c r="H6" t="n">
-        <v>55</v>
+        <v>8750</v>
       </c>
       <c r="I6" t="n">
-        <v>9</v>
+        <v>283</v>
       </c>
       <c r="J6" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="K6" t="n">
         <v>150</v>
@@ -712,36 +712,36 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>IN0012</t>
+          <t>IN0011</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Item 12</t>
+          <t>Item 11</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Descr 12</t>
+          <t>Descr 11</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="G7" t="n">
-        <v>22</v>
+        <v>176</v>
       </c>
       <c r="H7" t="n">
-        <v>396</v>
+        <v>10384</v>
       </c>
       <c r="I7" t="n">
-        <v>36</v>
+        <v>229</v>
       </c>
       <c r="J7" t="n">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="K7" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="L7" t="inlineStr"/>
       <c r="M7" t="inlineStr"/>
@@ -753,33 +753,33 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>IN0018</t>
+          <t>IN0016</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Item 18</t>
+          <t>Item 16</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Descr 18</t>
+          <t>Descr 16</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>12</v>
+        <v>90</v>
       </c>
       <c r="G8" t="n">
-        <v>6</v>
+        <v>96</v>
       </c>
       <c r="H8" t="n">
-        <v>72</v>
+        <v>8640</v>
       </c>
       <c r="I8" t="n">
-        <v>7</v>
+        <v>180</v>
       </c>
       <c r="J8" t="n">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="K8" t="n">
         <v>50</v>
@@ -794,38 +794,42 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>IN0025</t>
+          <t>IN0017</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Item 25</t>
+          <t>Item 17</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Descr 25</t>
+          <t>Descr 17</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>14</v>
+        <v>97</v>
       </c>
       <c r="G9" t="n">
-        <v>28</v>
+        <v>57</v>
       </c>
       <c r="H9" t="n">
-        <v>392</v>
+        <v>5529</v>
       </c>
       <c r="I9" t="n">
-        <v>21</v>
+        <v>98</v>
       </c>
       <c r="J9" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="K9" t="n">
         <v>50</v>
       </c>
-      <c r="L9" t="inlineStr"/>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
       <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
@@ -835,33 +839,33 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>IN0006</t>
+          <t>IN0019</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>Item 6</t>
+          <t>Item 19</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Descr 6</t>
+          <t>Descr 19</t>
         </is>
       </c>
       <c r="F10" t="n">
-        <v>11</v>
+        <v>82</v>
       </c>
       <c r="G10" t="n">
-        <v>5</v>
+        <v>143</v>
       </c>
       <c r="H10" t="n">
-        <v>55</v>
+        <v>11726</v>
       </c>
       <c r="I10" t="n">
-        <v>9</v>
+        <v>164</v>
       </c>
       <c r="J10" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K10" t="n">
         <v>150</v>
@@ -872,40 +876,40 @@
     <row r="11">
       <c r="A11" t="inlineStr"/>
       <c r="B11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>IN0012</t>
+          <t>IN0022</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Item 12</t>
+          <t>Item 22</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Descr 12</t>
+          <t>Descr 22</t>
         </is>
       </c>
       <c r="F11" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="G11" t="n">
-        <v>22</v>
+        <v>182</v>
       </c>
       <c r="H11" t="n">
-        <v>396</v>
+        <v>4368</v>
       </c>
       <c r="I11" t="n">
-        <v>36</v>
+        <v>132</v>
       </c>
       <c r="J11" t="n">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="K11" t="n">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="L11" t="inlineStr"/>
       <c r="M11" t="inlineStr"/>
@@ -913,40 +917,40 @@
     <row r="12">
       <c r="A12" t="inlineStr"/>
       <c r="B12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>IN0018</t>
+          <t>IN0024</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Item 18</t>
+          <t>Item 24</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Descr 18</t>
+          <t>Descr 24</t>
         </is>
       </c>
       <c r="F12" t="n">
-        <v>12</v>
+        <v>75</v>
       </c>
       <c r="G12" t="n">
-        <v>6</v>
+        <v>173</v>
       </c>
       <c r="H12" t="n">
-        <v>72</v>
+        <v>12975</v>
       </c>
       <c r="I12" t="n">
-        <v>7</v>
+        <v>127</v>
       </c>
       <c r="J12" t="n">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="K12" t="n">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="L12" t="inlineStr"/>
       <c r="M12" t="inlineStr"/>
@@ -954,43 +958,912 @@
     <row r="13">
       <c r="A13" t="inlineStr"/>
       <c r="B13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>IN0025</t>
+          <t>IN0002</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Item 25</t>
+          <t>Item 2</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Descr 25</t>
+          <t>Descr 2</t>
         </is>
       </c>
       <c r="F13" t="n">
-        <v>14</v>
+        <v>93</v>
       </c>
       <c r="G13" t="n">
-        <v>28</v>
+        <v>132</v>
       </c>
       <c r="H13" t="n">
-        <v>392</v>
+        <v>12276</v>
       </c>
       <c r="I13" t="n">
-        <v>21</v>
+        <v>231</v>
       </c>
       <c r="J13" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="K13" t="n">
         <v>50</v>
       </c>
       <c r="L13" t="inlineStr"/>
       <c r="M13" t="inlineStr"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr"/>
+      <c r="B14" t="n">
+        <v>0</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>IN0003</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Item 3</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Descr 3</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>57</v>
+      </c>
+      <c r="G14" t="n">
+        <v>151</v>
+      </c>
+      <c r="H14" t="n">
+        <v>8607</v>
+      </c>
+      <c r="I14" t="n">
+        <v>114</v>
+      </c>
+      <c r="J14" t="n">
+        <v>11</v>
+      </c>
+      <c r="K14" t="n">
+        <v>150</v>
+      </c>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr"/>
+      <c r="B15" t="n">
+        <v>0</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>IN0005</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Item 5</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Descr 5</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>75</v>
+      </c>
+      <c r="G15" t="n">
+        <v>62</v>
+      </c>
+      <c r="H15" t="n">
+        <v>4650</v>
+      </c>
+      <c r="I15" t="n">
+        <v>39</v>
+      </c>
+      <c r="J15" t="n">
+        <v>12</v>
+      </c>
+      <c r="K15" t="n">
+        <v>50</v>
+      </c>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr"/>
+      <c r="B16" t="n">
+        <v>0</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>IN0009</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Item 9</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Descr 9</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>59</v>
+      </c>
+      <c r="G16" t="n">
+        <v>122</v>
+      </c>
+      <c r="H16" t="n">
+        <v>7198</v>
+      </c>
+      <c r="I16" t="n">
+        <v>82</v>
+      </c>
+      <c r="J16" t="n">
+        <v>3</v>
+      </c>
+      <c r="K16" t="n">
+        <v>150</v>
+      </c>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr"/>
+      <c r="B17" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>IN0010</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Item 10</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Descr 10</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>50</v>
+      </c>
+      <c r="G17" t="n">
+        <v>175</v>
+      </c>
+      <c r="H17" t="n">
+        <v>8750</v>
+      </c>
+      <c r="I17" t="n">
+        <v>283</v>
+      </c>
+      <c r="J17" t="n">
+        <v>8</v>
+      </c>
+      <c r="K17" t="n">
+        <v>150</v>
+      </c>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+      <c r="B18" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>IN0011</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Item 11</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Descr 11</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>59</v>
+      </c>
+      <c r="G18" t="n">
+        <v>176</v>
+      </c>
+      <c r="H18" t="n">
+        <v>10384</v>
+      </c>
+      <c r="I18" t="n">
+        <v>229</v>
+      </c>
+      <c r="J18" t="n">
+        <v>1</v>
+      </c>
+      <c r="K18" t="n">
+        <v>100</v>
+      </c>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr"/>
+      <c r="B19" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>IN0016</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Item 16</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Descr 16</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>90</v>
+      </c>
+      <c r="G19" t="n">
+        <v>96</v>
+      </c>
+      <c r="H19" t="n">
+        <v>8640</v>
+      </c>
+      <c r="I19" t="n">
+        <v>180</v>
+      </c>
+      <c r="J19" t="n">
+        <v>3</v>
+      </c>
+      <c r="K19" t="n">
+        <v>50</v>
+      </c>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+      <c r="B20" t="n">
+        <v>0</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>IN0017</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Item 17</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Descr 17</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>97</v>
+      </c>
+      <c r="G20" t="n">
+        <v>57</v>
+      </c>
+      <c r="H20" t="n">
+        <v>5529</v>
+      </c>
+      <c r="I20" t="n">
+        <v>98</v>
+      </c>
+      <c r="J20" t="n">
+        <v>12</v>
+      </c>
+      <c r="K20" t="n">
+        <v>50</v>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr"/>
+      <c r="B21" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>IN0019</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Item 19</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Descr 19</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>82</v>
+      </c>
+      <c r="G21" t="n">
+        <v>143</v>
+      </c>
+      <c r="H21" t="n">
+        <v>11726</v>
+      </c>
+      <c r="I21" t="n">
+        <v>164</v>
+      </c>
+      <c r="J21" t="n">
+        <v>12</v>
+      </c>
+      <c r="K21" t="n">
+        <v>150</v>
+      </c>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr"/>
+      <c r="B22" t="n">
+        <v>0</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>IN0022</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Item 22</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Descr 22</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>24</v>
+      </c>
+      <c r="G22" t="n">
+        <v>182</v>
+      </c>
+      <c r="H22" t="n">
+        <v>4368</v>
+      </c>
+      <c r="I22" t="n">
+        <v>132</v>
+      </c>
+      <c r="J22" t="n">
+        <v>15</v>
+      </c>
+      <c r="K22" t="n">
+        <v>150</v>
+      </c>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr"/>
+      <c r="B23" t="n">
+        <v>0</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>IN0024</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Item 24</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Descr 24</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>75</v>
+      </c>
+      <c r="G23" t="n">
+        <v>173</v>
+      </c>
+      <c r="H23" t="n">
+        <v>12975</v>
+      </c>
+      <c r="I23" t="n">
+        <v>127</v>
+      </c>
+      <c r="J23" t="n">
+        <v>9</v>
+      </c>
+      <c r="K23" t="n">
+        <v>100</v>
+      </c>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr"/>
+      <c r="B24" t="n">
+        <v>1</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>IN0002</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Item 2</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Descr 2</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>93</v>
+      </c>
+      <c r="G24" t="n">
+        <v>132</v>
+      </c>
+      <c r="H24" t="n">
+        <v>12276</v>
+      </c>
+      <c r="I24" t="n">
+        <v>231</v>
+      </c>
+      <c r="J24" t="n">
+        <v>4</v>
+      </c>
+      <c r="K24" t="n">
+        <v>50</v>
+      </c>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr"/>
+      <c r="B25" t="n">
+        <v>0</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>IN0003</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Item 3</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Descr 3</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>57</v>
+      </c>
+      <c r="G25" t="n">
+        <v>151</v>
+      </c>
+      <c r="H25" t="n">
+        <v>8607</v>
+      </c>
+      <c r="I25" t="n">
+        <v>114</v>
+      </c>
+      <c r="J25" t="n">
+        <v>11</v>
+      </c>
+      <c r="K25" t="n">
+        <v>150</v>
+      </c>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+      <c r="B26" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>IN0005</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Item 5</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Descr 5</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>75</v>
+      </c>
+      <c r="G26" t="n">
+        <v>62</v>
+      </c>
+      <c r="H26" t="n">
+        <v>4650</v>
+      </c>
+      <c r="I26" t="n">
+        <v>39</v>
+      </c>
+      <c r="J26" t="n">
+        <v>12</v>
+      </c>
+      <c r="K26" t="n">
+        <v>50</v>
+      </c>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr"/>
+      <c r="B27" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>IN0009</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Item 9</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Descr 9</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>59</v>
+      </c>
+      <c r="G27" t="n">
+        <v>122</v>
+      </c>
+      <c r="H27" t="n">
+        <v>7198</v>
+      </c>
+      <c r="I27" t="n">
+        <v>82</v>
+      </c>
+      <c r="J27" t="n">
+        <v>3</v>
+      </c>
+      <c r="K27" t="n">
+        <v>150</v>
+      </c>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr"/>
+      <c r="B28" t="n">
+        <v>1</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>IN0010</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Item 10</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Descr 10</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>50</v>
+      </c>
+      <c r="G28" t="n">
+        <v>175</v>
+      </c>
+      <c r="H28" t="n">
+        <v>8750</v>
+      </c>
+      <c r="I28" t="n">
+        <v>283</v>
+      </c>
+      <c r="J28" t="n">
+        <v>8</v>
+      </c>
+      <c r="K28" t="n">
+        <v>150</v>
+      </c>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr"/>
+      <c r="B29" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>IN0011</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Item 11</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Descr 11</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>59</v>
+      </c>
+      <c r="G29" t="n">
+        <v>176</v>
+      </c>
+      <c r="H29" t="n">
+        <v>10384</v>
+      </c>
+      <c r="I29" t="n">
+        <v>229</v>
+      </c>
+      <c r="J29" t="n">
+        <v>1</v>
+      </c>
+      <c r="K29" t="n">
+        <v>100</v>
+      </c>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr"/>
+      <c r="B30" t="n">
+        <v>1</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>IN0016</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Item 16</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Descr 16</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>90</v>
+      </c>
+      <c r="G30" t="n">
+        <v>96</v>
+      </c>
+      <c r="H30" t="n">
+        <v>8640</v>
+      </c>
+      <c r="I30" t="n">
+        <v>180</v>
+      </c>
+      <c r="J30" t="n">
+        <v>3</v>
+      </c>
+      <c r="K30" t="n">
+        <v>50</v>
+      </c>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+      <c r="B31" t="n">
+        <v>0</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>IN0017</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Item 17</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Descr 17</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>97</v>
+      </c>
+      <c r="G31" t="n">
+        <v>57</v>
+      </c>
+      <c r="H31" t="n">
+        <v>5529</v>
+      </c>
+      <c r="I31" t="n">
+        <v>98</v>
+      </c>
+      <c r="J31" t="n">
+        <v>12</v>
+      </c>
+      <c r="K31" t="n">
+        <v>50</v>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr"/>
+      <c r="B32" t="n">
+        <v>1</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>IN0019</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Item 19</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Descr 19</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>82</v>
+      </c>
+      <c r="G32" t="n">
+        <v>143</v>
+      </c>
+      <c r="H32" t="n">
+        <v>11726</v>
+      </c>
+      <c r="I32" t="n">
+        <v>164</v>
+      </c>
+      <c r="J32" t="n">
+        <v>12</v>
+      </c>
+      <c r="K32" t="n">
+        <v>150</v>
+      </c>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr"/>
+      <c r="B33" t="n">
+        <v>0</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>IN0022</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Item 22</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Descr 22</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>24</v>
+      </c>
+      <c r="G33" t="n">
+        <v>182</v>
+      </c>
+      <c r="H33" t="n">
+        <v>4368</v>
+      </c>
+      <c r="I33" t="n">
+        <v>132</v>
+      </c>
+      <c r="J33" t="n">
+        <v>15</v>
+      </c>
+      <c r="K33" t="n">
+        <v>150</v>
+      </c>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr"/>
+      <c r="B34" t="n">
+        <v>0</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>IN0024</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Item 24</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Descr 24</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>75</v>
+      </c>
+      <c r="G34" t="n">
+        <v>173</v>
+      </c>
+      <c r="H34" t="n">
+        <v>12975</v>
+      </c>
+      <c r="I34" t="n">
+        <v>127</v>
+      </c>
+      <c r="J34" t="n">
+        <v>9</v>
+      </c>
+      <c r="K34" t="n">
+        <v>100</v>
+      </c>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
atualizado local do projeto, aguardando planilhas a serem consolidadas
</commit_message>
<xml_diff>
--- a/relatórios/relatorio.xlsx
+++ b/relatórios/relatorio.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:M13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -548,36 +548,36 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>IN0006</t>
+          <t>IN0012</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Item 6</t>
+          <t>Item 12</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Descr 6</t>
+          <t>Descr 12</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G3" t="n">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="H3" t="n">
-        <v>55</v>
+        <v>396</v>
       </c>
       <c r="I3" t="n">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="J3" t="n">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K3" t="n">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="L3" t="inlineStr"/>
       <c r="M3" t="inlineStr"/>
@@ -589,39 +589,408 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>IN0006</t>
+          <t>IN0018</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Item 6</t>
+          <t>Item 18</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Descr 6</t>
+          <t>Descr 18</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G4" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H4" t="n">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="I4" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="J4" t="n">
         <v>13</v>
       </c>
       <c r="K4" t="n">
-        <v>150</v>
+        <v>50</v>
       </c>
       <c r="L4" t="inlineStr"/>
       <c r="M4" t="inlineStr"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>IN0025</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Item 25</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Descr 25</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>14</v>
+      </c>
+      <c r="G5" t="n">
+        <v>28</v>
+      </c>
+      <c r="H5" t="n">
+        <v>392</v>
+      </c>
+      <c r="I5" t="n">
+        <v>21</v>
+      </c>
+      <c r="J5" t="n">
+        <v>8</v>
+      </c>
+      <c r="K5" t="n">
+        <v>50</v>
+      </c>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>IN0006</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Item 6</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Descr 6</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>11</v>
+      </c>
+      <c r="G6" t="n">
+        <v>5</v>
+      </c>
+      <c r="H6" t="n">
+        <v>55</v>
+      </c>
+      <c r="I6" t="n">
+        <v>9</v>
+      </c>
+      <c r="J6" t="n">
+        <v>13</v>
+      </c>
+      <c r="K6" t="n">
+        <v>150</v>
+      </c>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>IN0012</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Item 12</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>Descr 12</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>18</v>
+      </c>
+      <c r="G7" t="n">
+        <v>22</v>
+      </c>
+      <c r="H7" t="n">
+        <v>396</v>
+      </c>
+      <c r="I7" t="n">
+        <v>36</v>
+      </c>
+      <c r="J7" t="n">
+        <v>12</v>
+      </c>
+      <c r="K7" t="n">
+        <v>50</v>
+      </c>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr"/>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>IN0018</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Item 18</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>Descr 18</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>12</v>
+      </c>
+      <c r="G8" t="n">
+        <v>6</v>
+      </c>
+      <c r="H8" t="n">
+        <v>72</v>
+      </c>
+      <c r="I8" t="n">
+        <v>7</v>
+      </c>
+      <c r="J8" t="n">
+        <v>13</v>
+      </c>
+      <c r="K8" t="n">
+        <v>50</v>
+      </c>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr"/>
+      <c r="B9" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>IN0025</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Item 25</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Descr 25</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>14</v>
+      </c>
+      <c r="G9" t="n">
+        <v>28</v>
+      </c>
+      <c r="H9" t="n">
+        <v>392</v>
+      </c>
+      <c r="I9" t="n">
+        <v>21</v>
+      </c>
+      <c r="J9" t="n">
+        <v>8</v>
+      </c>
+      <c r="K9" t="n">
+        <v>50</v>
+      </c>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr"/>
+      <c r="B10" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>IN0006</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Item 6</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Descr 6</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>11</v>
+      </c>
+      <c r="G10" t="n">
+        <v>5</v>
+      </c>
+      <c r="H10" t="n">
+        <v>55</v>
+      </c>
+      <c r="I10" t="n">
+        <v>9</v>
+      </c>
+      <c r="J10" t="n">
+        <v>13</v>
+      </c>
+      <c r="K10" t="n">
+        <v>150</v>
+      </c>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr"/>
+      <c r="B11" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>IN0012</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Item 12</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Descr 12</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>18</v>
+      </c>
+      <c r="G11" t="n">
+        <v>22</v>
+      </c>
+      <c r="H11" t="n">
+        <v>396</v>
+      </c>
+      <c r="I11" t="n">
+        <v>36</v>
+      </c>
+      <c r="J11" t="n">
+        <v>12</v>
+      </c>
+      <c r="K11" t="n">
+        <v>50</v>
+      </c>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+      <c r="B12" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>IN0018</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Item 18</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Descr 18</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>12</v>
+      </c>
+      <c r="G12" t="n">
+        <v>6</v>
+      </c>
+      <c r="H12" t="n">
+        <v>72</v>
+      </c>
+      <c r="I12" t="n">
+        <v>7</v>
+      </c>
+      <c r="J12" t="n">
+        <v>13</v>
+      </c>
+      <c r="K12" t="n">
+        <v>50</v>
+      </c>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr"/>
+      <c r="B13" t="n">
+        <v>0</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>IN0025</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Item 25</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Descr 25</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>14</v>
+      </c>
+      <c r="G13" t="n">
+        <v>28</v>
+      </c>
+      <c r="H13" t="n">
+        <v>392</v>
+      </c>
+      <c r="I13" t="n">
+        <v>21</v>
+      </c>
+      <c r="J13" t="n">
+        <v>8</v>
+      </c>
+      <c r="K13" t="n">
+        <v>50</v>
+      </c>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>